<commit_message>
Weekly update: Latest gameweek results
</commit_message>
<xml_diff>
--- a/data/lineup_data.xlsx
+++ b/data/lineup_data.xlsx
@@ -17,16 +17,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="1">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -37,7 +34,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -45,21 +42,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -434,47 +422,47 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" t="inlineStr">
         <is>
           <t>Manager</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" t="inlineStr">
         <is>
           <t>Team Name</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" t="inlineStr">
         <is>
           <t>Position</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="D1" t="inlineStr">
         <is>
           <t>Player</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="E1" t="inlineStr">
         <is>
           <t>Position Type</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>GW 23 Score</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>GW 24 Score</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
         <is>
           <t>Is Captain</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>Is Vice Captain</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>Multiplier</t>
         </is>
@@ -505,7 +493,7 @@
         </is>
       </c>
       <c r="F2" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="G2" t="b">
         <v>0</v>
@@ -542,7 +530,7 @@
         </is>
       </c>
       <c r="F3" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="G3" t="b">
         <v>0</v>
@@ -579,7 +567,7 @@
         </is>
       </c>
       <c r="F4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G4" t="b">
         <v>0</v>
@@ -616,7 +604,7 @@
         </is>
       </c>
       <c r="F5" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="G5" t="b">
         <v>0</v>
@@ -653,7 +641,7 @@
         </is>
       </c>
       <c r="F6" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="G6" t="b">
         <v>0</v>
@@ -690,7 +678,7 @@
         </is>
       </c>
       <c r="F7" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G7" t="b">
         <v>0</v>
@@ -727,7 +715,7 @@
         </is>
       </c>
       <c r="F8" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="G8" t="b">
         <v>0</v>
@@ -764,7 +752,7 @@
         </is>
       </c>
       <c r="F9" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G9" t="b">
         <v>0</v>
@@ -801,7 +789,7 @@
         </is>
       </c>
       <c r="F10" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G10" t="b">
         <v>0</v>
@@ -912,7 +900,7 @@
         </is>
       </c>
       <c r="F13" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G13" t="b">
         <v>0</v>
@@ -986,7 +974,7 @@
         </is>
       </c>
       <c r="F15" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="G15" t="b">
         <v>0</v>
@@ -1060,7 +1048,7 @@
         </is>
       </c>
       <c r="F17" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="G17" t="b">
         <v>0</v>
@@ -1097,7 +1085,7 @@
         </is>
       </c>
       <c r="F18" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="G18" t="b">
         <v>0</v>
@@ -1134,7 +1122,7 @@
         </is>
       </c>
       <c r="F19" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="G19" t="b">
         <v>0</v>
@@ -1171,7 +1159,7 @@
         </is>
       </c>
       <c r="F20" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="G20" t="b">
         <v>0</v>
@@ -1208,7 +1196,7 @@
         </is>
       </c>
       <c r="F21" t="n">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="G21" t="b">
         <v>0</v>
@@ -1282,7 +1270,7 @@
         </is>
       </c>
       <c r="F23" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G23" t="b">
         <v>0</v>
@@ -1319,7 +1307,7 @@
         </is>
       </c>
       <c r="F24" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G24" t="b">
         <v>0</v>
@@ -1356,7 +1344,7 @@
         </is>
       </c>
       <c r="F25" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="G25" t="b">
         <v>0</v>
@@ -1393,7 +1381,7 @@
         </is>
       </c>
       <c r="F26" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G26" t="b">
         <v>1</v>
@@ -1467,7 +1455,7 @@
         </is>
       </c>
       <c r="F28" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G28" t="b">
         <v>0</v>
@@ -1541,7 +1529,7 @@
         </is>
       </c>
       <c r="F30" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="G30" t="b">
         <v>0</v>
@@ -1578,7 +1566,7 @@
         </is>
       </c>
       <c r="F31" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G31" t="b">
         <v>0</v>
@@ -1615,7 +1603,7 @@
         </is>
       </c>
       <c r="F32" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="G32" t="b">
         <v>0</v>
@@ -1643,7 +1631,7 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Virgil</t>
+          <t>Tarkowski</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
@@ -1652,7 +1640,7 @@
         </is>
       </c>
       <c r="F33" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="G33" t="b">
         <v>0</v>
@@ -1689,7 +1677,7 @@
         </is>
       </c>
       <c r="F34" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G34" t="b">
         <v>0</v>
@@ -1726,7 +1714,7 @@
         </is>
       </c>
       <c r="F35" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="G35" t="b">
         <v>0</v>
@@ -1763,7 +1751,7 @@
         </is>
       </c>
       <c r="F36" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="G36" t="b">
         <v>0</v>
@@ -1800,7 +1788,7 @@
         </is>
       </c>
       <c r="F37" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="G37" t="b">
         <v>0</v>
@@ -1837,7 +1825,7 @@
         </is>
       </c>
       <c r="F38" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G38" t="b">
         <v>0</v>
@@ -1865,7 +1853,7 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Reijnders</t>
+          <t>Wirtz</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
@@ -1874,7 +1862,7 @@
         </is>
       </c>
       <c r="F39" t="n">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="G39" t="b">
         <v>0</v>
@@ -1911,7 +1899,7 @@
         </is>
       </c>
       <c r="F40" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G40" t="b">
         <v>1</v>
@@ -1985,7 +1973,7 @@
         </is>
       </c>
       <c r="F42" t="n">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="G42" t="b">
         <v>0</v>
@@ -2022,7 +2010,7 @@
         </is>
       </c>
       <c r="F43" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G43" t="b">
         <v>0</v>
@@ -2050,7 +2038,7 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>Enzo</t>
+          <t>Amad</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
@@ -2059,7 +2047,7 @@
         </is>
       </c>
       <c r="F44" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="G44" t="b">
         <v>0</v>
@@ -2087,16 +2075,16 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>Tarkowski</t>
+          <t>Reijnders</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>DEF</t>
+          <t>MID</t>
         </is>
       </c>
       <c r="F45" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G45" t="b">
         <v>0</v>
@@ -2124,16 +2112,16 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>Grealish</t>
+          <t>Collins</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>MID</t>
+          <t>DEF</t>
         </is>
       </c>
       <c r="F46" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G46" t="b">
         <v>0</v>
@@ -2170,7 +2158,7 @@
         </is>
       </c>
       <c r="F47" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G47" t="b">
         <v>0</v>
@@ -2198,7 +2186,7 @@
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>Guéhi</t>
+          <t>Senesi</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
@@ -2207,7 +2195,7 @@
         </is>
       </c>
       <c r="F48" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G48" t="b">
         <v>0</v>
@@ -2244,7 +2232,7 @@
         </is>
       </c>
       <c r="F49" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G49" t="b">
         <v>0</v>
@@ -2281,7 +2269,7 @@
         </is>
       </c>
       <c r="F50" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="G50" t="b">
         <v>0</v>
@@ -2309,7 +2297,7 @@
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>Tarkowski</t>
+          <t>Guéhi</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
@@ -2318,7 +2306,7 @@
         </is>
       </c>
       <c r="F51" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G51" t="b">
         <v>0</v>
@@ -2392,7 +2380,7 @@
         </is>
       </c>
       <c r="F53" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G53" t="b">
         <v>0</v>
@@ -2429,7 +2417,7 @@
         </is>
       </c>
       <c r="F54" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G54" t="b">
         <v>0</v>
@@ -2457,7 +2445,7 @@
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>Ndiaye</t>
+          <t>B.Fernandes</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
@@ -2466,16 +2454,16 @@
         </is>
       </c>
       <c r="F55" t="n">
+        <v>10</v>
+      </c>
+      <c r="G55" t="b">
+        <v>1</v>
+      </c>
+      <c r="H55" t="b">
+        <v>0</v>
+      </c>
+      <c r="I55" t="n">
         <v>2</v>
-      </c>
-      <c r="G55" t="b">
-        <v>0</v>
-      </c>
-      <c r="H55" t="b">
-        <v>0</v>
-      </c>
-      <c r="I55" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="56">
@@ -2494,25 +2482,25 @@
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>Haaland</t>
+          <t>Ndiaye</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>FWD</t>
+          <t>MID</t>
         </is>
       </c>
       <c r="F56" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G56" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H56" t="b">
         <v>0</v>
       </c>
       <c r="I56" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="57">
@@ -2531,7 +2519,7 @@
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>Thiago</t>
+          <t>Haaland</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
@@ -2540,7 +2528,7 @@
         </is>
       </c>
       <c r="F57" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G57" t="b">
         <v>0</v>
@@ -2577,7 +2565,7 @@
         </is>
       </c>
       <c r="F58" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G58" t="b">
         <v>0</v>
@@ -2605,16 +2593,16 @@
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>B.Fernandes</t>
+          <t>Tarkowski</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>MID</t>
+          <t>DEF</t>
         </is>
       </c>
       <c r="F59" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G59" t="b">
         <v>0</v>
@@ -2642,16 +2630,16 @@
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>Senesi</t>
+          <t>Thiago</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>DEF</t>
+          <t>FWD</t>
         </is>
       </c>
       <c r="F60" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G60" t="b">
         <v>0</v>
@@ -2716,7 +2704,7 @@
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>Verbruggen</t>
+          <t>Dúbravka</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
@@ -2753,7 +2741,7 @@
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>Chalobah</t>
+          <t>Gabriel</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
@@ -2762,7 +2750,7 @@
         </is>
       </c>
       <c r="F63" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="G63" t="b">
         <v>0</v>
@@ -2790,7 +2778,7 @@
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>Guéhi</t>
+          <t>Senesi</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
@@ -2799,7 +2787,7 @@
         </is>
       </c>
       <c r="F64" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G64" t="b">
         <v>0</v>
@@ -2827,7 +2815,7 @@
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>Gabriel</t>
+          <t>Guéhi</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
@@ -2836,7 +2824,7 @@
         </is>
       </c>
       <c r="F65" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G65" t="b">
         <v>0</v>
@@ -2864,16 +2852,16 @@
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>Rice</t>
+          <t>Chalobah</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>MID</t>
+          <t>DEF</t>
         </is>
       </c>
       <c r="F66" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G66" t="b">
         <v>0</v>
@@ -2901,7 +2889,7 @@
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>Foden</t>
+          <t>Semenyo</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
@@ -2910,7 +2898,7 @@
         </is>
       </c>
       <c r="F67" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="G67" t="b">
         <v>0</v>
@@ -2938,7 +2926,7 @@
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>Saka</t>
+          <t>B.Fernandes</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
@@ -2947,16 +2935,16 @@
         </is>
       </c>
       <c r="F68" t="n">
+        <v>10</v>
+      </c>
+      <c r="G68" t="b">
+        <v>1</v>
+      </c>
+      <c r="H68" t="b">
+        <v>0</v>
+      </c>
+      <c r="I68" t="n">
         <v>2</v>
-      </c>
-      <c r="G68" t="b">
-        <v>0</v>
-      </c>
-      <c r="H68" t="b">
-        <v>1</v>
-      </c>
-      <c r="I68" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="69">
@@ -2975,7 +2963,7 @@
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>Semenyo</t>
+          <t>Wilson</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
@@ -2984,7 +2972,7 @@
         </is>
       </c>
       <c r="F69" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="G69" t="b">
         <v>0</v>
@@ -3012,7 +3000,7 @@
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>Wilson</t>
+          <t>Rice</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
@@ -3021,7 +3009,7 @@
         </is>
       </c>
       <c r="F70" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="G70" t="b">
         <v>0</v>
@@ -3049,7 +3037,7 @@
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>Haaland</t>
+          <t>Thiago</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
@@ -3058,16 +3046,16 @@
         </is>
       </c>
       <c r="F71" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G71" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H71" t="b">
         <v>0</v>
       </c>
       <c r="I71" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="72">
@@ -3086,7 +3074,7 @@
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>Thiago</t>
+          <t>Haaland</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
@@ -3095,13 +3083,13 @@
         </is>
       </c>
       <c r="F72" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G72" t="b">
         <v>0</v>
       </c>
       <c r="H72" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I72" t="n">
         <v>1</v>
@@ -3123,7 +3111,7 @@
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>Dúbravka</t>
+          <t>Verbruggen</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
@@ -3132,7 +3120,7 @@
         </is>
       </c>
       <c r="F73" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G73" t="b">
         <v>0</v>
@@ -3160,16 +3148,16 @@
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>O'Reilly</t>
+          <t>Saka</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>DEF</t>
+          <t>MID</t>
         </is>
       </c>
       <c r="F74" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="G74" t="b">
         <v>0</v>
@@ -3197,7 +3185,7 @@
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>Senesi</t>
+          <t>Dorgu</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
@@ -3206,7 +3194,7 @@
         </is>
       </c>
       <c r="F75" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G75" t="b">
         <v>0</v>
@@ -3271,7 +3259,7 @@
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>Dúbravka</t>
+          <t>Petrović</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
@@ -3280,7 +3268,7 @@
         </is>
       </c>
       <c r="F77" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="G77" t="b">
         <v>0</v>
@@ -3317,7 +3305,7 @@
         </is>
       </c>
       <c r="F78" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G78" t="b">
         <v>0</v>
@@ -3354,7 +3342,7 @@
         </is>
       </c>
       <c r="F79" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G79" t="b">
         <v>0</v>
@@ -3382,7 +3370,7 @@
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>Guéhi</t>
+          <t>Senesi</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
@@ -3391,7 +3379,7 @@
         </is>
       </c>
       <c r="F80" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G80" t="b">
         <v>0</v>
@@ -3419,7 +3407,7 @@
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>Foden</t>
+          <t>Cunha</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
@@ -3428,7 +3416,7 @@
         </is>
       </c>
       <c r="F81" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="G81" t="b">
         <v>0</v>
@@ -3465,7 +3453,7 @@
         </is>
       </c>
       <c r="F82" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="G82" t="b">
         <v>0</v>
@@ -3502,7 +3490,7 @@
         </is>
       </c>
       <c r="F83" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="G83" t="b">
         <v>0</v>
@@ -3539,7 +3527,7 @@
         </is>
       </c>
       <c r="F84" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="G84" t="b">
         <v>0</v>
@@ -3576,7 +3564,7 @@
         </is>
       </c>
       <c r="F85" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G85" t="b">
         <v>0</v>
@@ -3650,7 +3638,7 @@
         </is>
       </c>
       <c r="F87" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G87" t="b">
         <v>1</v>
@@ -3678,7 +3666,7 @@
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>Petrović</t>
+          <t>Dúbravka</t>
         </is>
       </c>
       <c r="E88" t="inlineStr">
@@ -3715,12 +3703,12 @@
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>Neto</t>
+          <t>Guéhi</t>
         </is>
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>MID</t>
+          <t>DEF</t>
         </is>
       </c>
       <c r="F89" t="n">
@@ -3761,7 +3749,7 @@
         </is>
       </c>
       <c r="F90" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="G90" t="b">
         <v>0</v>
@@ -3789,16 +3777,16 @@
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>Senesi</t>
+          <t>Neto</t>
         </is>
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>DEF</t>
+          <t>MID</t>
         </is>
       </c>
       <c r="F91" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G91" t="b">
         <v>0</v>
@@ -3835,7 +3823,7 @@
         </is>
       </c>
       <c r="F92" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="G92" t="b">
         <v>0</v>
@@ -3872,7 +3860,7 @@
         </is>
       </c>
       <c r="F93" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="G93" t="b">
         <v>0</v>
@@ -3909,7 +3897,7 @@
         </is>
       </c>
       <c r="F94" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G94" t="b">
         <v>0</v>
@@ -3946,7 +3934,7 @@
         </is>
       </c>
       <c r="F95" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="G95" t="b">
         <v>0</v>
@@ -3974,16 +3962,16 @@
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>Zubimendi</t>
+          <t>Senesi</t>
         </is>
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>MID</t>
+          <t>DEF</t>
         </is>
       </c>
       <c r="F96" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="G96" t="b">
         <v>0</v>
@@ -4020,7 +4008,7 @@
         </is>
       </c>
       <c r="F97" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="G97" t="b">
         <v>0</v>
@@ -4048,7 +4036,7 @@
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>Cherki</t>
+          <t>Cunha</t>
         </is>
       </c>
       <c r="E98" t="inlineStr">
@@ -4057,7 +4045,7 @@
         </is>
       </c>
       <c r="F98" t="n">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="G98" t="b">
         <v>0</v>
@@ -4094,7 +4082,7 @@
         </is>
       </c>
       <c r="F99" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G99" t="b">
         <v>0</v>
@@ -4131,7 +4119,7 @@
         </is>
       </c>
       <c r="F100" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G100" t="b">
         <v>1</v>
@@ -4159,7 +4147,7 @@
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>Ekitiké</t>
+          <t>João Pedro</t>
         </is>
       </c>
       <c r="E101" t="inlineStr">
@@ -4168,7 +4156,7 @@
         </is>
       </c>
       <c r="F101" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="G101" t="b">
         <v>0</v>
@@ -4242,7 +4230,7 @@
         </is>
       </c>
       <c r="F103" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G103" t="b">
         <v>0</v>
@@ -4270,7 +4258,7 @@
       </c>
       <c r="D104" t="inlineStr">
         <is>
-          <t>Cunha</t>
+          <t>Zubimendi</t>
         </is>
       </c>
       <c r="E104" t="inlineStr">
@@ -4279,7 +4267,7 @@
         </is>
       </c>
       <c r="F104" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G104" t="b">
         <v>0</v>
@@ -4307,16 +4295,16 @@
       </c>
       <c r="D105" t="inlineStr">
         <is>
-          <t>Senesi</t>
+          <t>Cherki</t>
         </is>
       </c>
       <c r="E105" t="inlineStr">
         <is>
-          <t>DEF</t>
+          <t>MID</t>
         </is>
       </c>
       <c r="F105" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="G105" t="b">
         <v>0</v>
@@ -4353,7 +4341,7 @@
         </is>
       </c>
       <c r="F106" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="G106" t="b">
         <v>0</v>
@@ -4390,7 +4378,7 @@
         </is>
       </c>
       <c r="F107" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="G107" t="b">
         <v>0</v>
@@ -4418,7 +4406,7 @@
       </c>
       <c r="D108" t="inlineStr">
         <is>
-          <t>Tarkowski</t>
+          <t>Chalobah</t>
         </is>
       </c>
       <c r="E108" t="inlineStr">
@@ -4427,7 +4415,7 @@
         </is>
       </c>
       <c r="F108" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G108" t="b">
         <v>0</v>
@@ -4455,7 +4443,7 @@
       </c>
       <c r="D109" t="inlineStr">
         <is>
-          <t>Chalobah</t>
+          <t>Tarkowski</t>
         </is>
       </c>
       <c r="E109" t="inlineStr">
@@ -4464,7 +4452,7 @@
         </is>
       </c>
       <c r="F109" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G109" t="b">
         <v>0</v>
@@ -4492,7 +4480,7 @@
       </c>
       <c r="D110" t="inlineStr">
         <is>
-          <t>Guéhi</t>
+          <t>J.Timber</t>
         </is>
       </c>
       <c r="E110" t="inlineStr">
@@ -4501,7 +4489,7 @@
         </is>
       </c>
       <c r="F110" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G110" t="b">
         <v>0</v>
@@ -4529,7 +4517,7 @@
       </c>
       <c r="D111" t="inlineStr">
         <is>
-          <t>J.Timber</t>
+          <t>Alderete</t>
         </is>
       </c>
       <c r="E111" t="inlineStr">
@@ -4538,7 +4526,7 @@
         </is>
       </c>
       <c r="F111" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="G111" t="b">
         <v>0</v>
@@ -4566,7 +4554,7 @@
       </c>
       <c r="D112" t="inlineStr">
         <is>
-          <t>Rice</t>
+          <t>Rogers</t>
         </is>
       </c>
       <c r="E112" t="inlineStr">
@@ -4575,7 +4563,7 @@
         </is>
       </c>
       <c r="F112" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G112" t="b">
         <v>0</v>
@@ -4603,7 +4591,7 @@
       </c>
       <c r="D113" t="inlineStr">
         <is>
-          <t>Rogers</t>
+          <t>Enzo</t>
         </is>
       </c>
       <c r="E113" t="inlineStr">
@@ -4640,7 +4628,7 @@
       </c>
       <c r="D114" t="inlineStr">
         <is>
-          <t>Semenyo</t>
+          <t>Rice</t>
         </is>
       </c>
       <c r="E114" t="inlineStr">
@@ -4649,7 +4637,7 @@
         </is>
       </c>
       <c r="F114" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="G114" t="b">
         <v>0</v>
@@ -4677,25 +4665,25 @@
       </c>
       <c r="D115" t="inlineStr">
         <is>
-          <t>Haaland</t>
+          <t>Semenyo</t>
         </is>
       </c>
       <c r="E115" t="inlineStr">
         <is>
-          <t>FWD</t>
+          <t>MID</t>
         </is>
       </c>
       <c r="F115" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="G115" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H115" t="b">
         <v>0</v>
       </c>
       <c r="I115" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="116">
@@ -4714,7 +4702,7 @@
       </c>
       <c r="D116" t="inlineStr">
         <is>
-          <t>Thiago</t>
+          <t>Haaland</t>
         </is>
       </c>
       <c r="E116" t="inlineStr">
@@ -4723,16 +4711,16 @@
         </is>
       </c>
       <c r="F116" t="n">
+        <v>5</v>
+      </c>
+      <c r="G116" t="b">
+        <v>1</v>
+      </c>
+      <c r="H116" t="b">
+        <v>0</v>
+      </c>
+      <c r="I116" t="n">
         <v>2</v>
-      </c>
-      <c r="G116" t="b">
-        <v>0</v>
-      </c>
-      <c r="H116" t="b">
-        <v>1</v>
-      </c>
-      <c r="I116" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="117">
@@ -4751,7 +4739,7 @@
       </c>
       <c r="D117" t="inlineStr">
         <is>
-          <t>Bowen</t>
+          <t>João Pedro</t>
         </is>
       </c>
       <c r="E117" t="inlineStr">
@@ -4760,13 +4748,13 @@
         </is>
       </c>
       <c r="F117" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G117" t="b">
         <v>0</v>
       </c>
       <c r="H117" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I117" t="n">
         <v>1</v>
@@ -4797,7 +4785,7 @@
         </is>
       </c>
       <c r="F118" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G118" t="b">
         <v>0</v>
@@ -4806,7 +4794,7 @@
         <v>0</v>
       </c>
       <c r="I118" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="119">
@@ -4825,16 +4813,16 @@
       </c>
       <c r="D119" t="inlineStr">
         <is>
-          <t>Bruno G.</t>
+          <t>Thiago</t>
         </is>
       </c>
       <c r="E119" t="inlineStr">
         <is>
-          <t>MID</t>
+          <t>FWD</t>
         </is>
       </c>
       <c r="F119" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G119" t="b">
         <v>0</v>
@@ -4843,7 +4831,7 @@
         <v>0</v>
       </c>
       <c r="I119" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="120">
@@ -4862,7 +4850,7 @@
       </c>
       <c r="D120" t="inlineStr">
         <is>
-          <t>Gravenberch</t>
+          <t>Bruno G.</t>
         </is>
       </c>
       <c r="E120" t="inlineStr">
@@ -4871,7 +4859,7 @@
         </is>
       </c>
       <c r="F120" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G120" t="b">
         <v>0</v>
@@ -4880,7 +4868,7 @@
         <v>0</v>
       </c>
       <c r="I120" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="121">
@@ -4899,7 +4887,7 @@
       </c>
       <c r="D121" t="inlineStr">
         <is>
-          <t>Alderete</t>
+          <t>Van de Ven</t>
         </is>
       </c>
       <c r="E121" t="inlineStr">
@@ -4908,7 +4896,7 @@
         </is>
       </c>
       <c r="F121" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G121" t="b">
         <v>0</v>
@@ -4917,7 +4905,7 @@
         <v>0</v>
       </c>
       <c r="I121" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="122">
@@ -4945,7 +4933,7 @@
         </is>
       </c>
       <c r="F122" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G122" t="b">
         <v>0</v>
@@ -4982,7 +4970,7 @@
         </is>
       </c>
       <c r="F123" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G123" t="b">
         <v>0</v>
@@ -5019,7 +5007,7 @@
         </is>
       </c>
       <c r="F124" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G124" t="b">
         <v>0</v>
@@ -5056,7 +5044,7 @@
         </is>
       </c>
       <c r="F125" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G125" t="b">
         <v>0</v>
@@ -5084,7 +5072,7 @@
       </c>
       <c r="D126" t="inlineStr">
         <is>
-          <t>Rodon</t>
+          <t>Keane</t>
         </is>
       </c>
       <c r="E126" t="inlineStr">
@@ -5093,7 +5081,7 @@
         </is>
       </c>
       <c r="F126" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G126" t="b">
         <v>0</v>
@@ -5167,7 +5155,7 @@
         </is>
       </c>
       <c r="F128" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G128" t="b">
         <v>0</v>
@@ -5204,7 +5192,7 @@
         </is>
       </c>
       <c r="F129" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="G129" t="b">
         <v>0</v>
@@ -5241,7 +5229,7 @@
         </is>
       </c>
       <c r="F130" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G130" t="b">
         <v>1</v>
@@ -5278,7 +5266,7 @@
         </is>
       </c>
       <c r="F131" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G131" t="b">
         <v>0</v>
@@ -5352,7 +5340,7 @@
         </is>
       </c>
       <c r="F133" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G133" t="b">
         <v>0</v>
@@ -5380,12 +5368,12 @@
       </c>
       <c r="D134" t="inlineStr">
         <is>
-          <t>Keane</t>
+          <t>Bruno G.</t>
         </is>
       </c>
       <c r="E134" t="inlineStr">
         <is>
-          <t>DEF</t>
+          <t>MID</t>
         </is>
       </c>
       <c r="F134" t="n">
@@ -5417,16 +5405,16 @@
       </c>
       <c r="D135" t="inlineStr">
         <is>
-          <t>Bruno G.</t>
+          <t>Rodon</t>
         </is>
       </c>
       <c r="E135" t="inlineStr">
         <is>
-          <t>MID</t>
+          <t>DEF</t>
         </is>
       </c>
       <c r="F135" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G135" t="b">
         <v>0</v>
@@ -5463,7 +5451,7 @@
         </is>
       </c>
       <c r="F136" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G136" t="b">
         <v>0</v>
@@ -5500,7 +5488,7 @@
         </is>
       </c>
       <c r="F137" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="G137" t="b">
         <v>0</v>
@@ -5528,7 +5516,7 @@
       </c>
       <c r="D138" t="inlineStr">
         <is>
-          <t>Tarkowski</t>
+          <t>Gabriel</t>
         </is>
       </c>
       <c r="E138" t="inlineStr">
@@ -5537,7 +5525,7 @@
         </is>
       </c>
       <c r="F138" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="G138" t="b">
         <v>0</v>
@@ -5565,7 +5553,7 @@
       </c>
       <c r="D139" t="inlineStr">
         <is>
-          <t>Gabriel</t>
+          <t>Tarkowski</t>
         </is>
       </c>
       <c r="E139" t="inlineStr">
@@ -5574,7 +5562,7 @@
         </is>
       </c>
       <c r="F139" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G139" t="b">
         <v>0</v>
@@ -5602,7 +5590,7 @@
       </c>
       <c r="D140" t="inlineStr">
         <is>
-          <t>Guéhi</t>
+          <t>Mukiele</t>
         </is>
       </c>
       <c r="E140" t="inlineStr">
@@ -5611,7 +5599,7 @@
         </is>
       </c>
       <c r="F140" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="G140" t="b">
         <v>0</v>
@@ -5639,7 +5627,7 @@
       </c>
       <c r="D141" t="inlineStr">
         <is>
-          <t>Ndiaye</t>
+          <t>Rice</t>
         </is>
       </c>
       <c r="E141" t="inlineStr">
@@ -5648,7 +5636,7 @@
         </is>
       </c>
       <c r="F141" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G141" t="b">
         <v>0</v>
@@ -5676,7 +5664,7 @@
       </c>
       <c r="D142" t="inlineStr">
         <is>
-          <t>Rice</t>
+          <t>Ndiaye</t>
         </is>
       </c>
       <c r="E142" t="inlineStr">
@@ -5685,7 +5673,7 @@
         </is>
       </c>
       <c r="F142" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G142" t="b">
         <v>0</v>
@@ -5722,7 +5710,7 @@
         </is>
       </c>
       <c r="F143" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="G143" t="b">
         <v>0</v>
@@ -5750,7 +5738,7 @@
       </c>
       <c r="D144" t="inlineStr">
         <is>
-          <t>Semenyo</t>
+          <t>B.Fernandes</t>
         </is>
       </c>
       <c r="E144" t="inlineStr">
@@ -5759,13 +5747,13 @@
         </is>
       </c>
       <c r="F144" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G144" t="b">
         <v>0</v>
       </c>
       <c r="H144" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I144" t="n">
         <v>1</v>
@@ -5787,25 +5775,25 @@
       </c>
       <c r="D145" t="inlineStr">
         <is>
-          <t>Haaland</t>
+          <t>Semenyo</t>
         </is>
       </c>
       <c r="E145" t="inlineStr">
         <is>
-          <t>FWD</t>
+          <t>MID</t>
         </is>
       </c>
       <c r="F145" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="G145" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H145" t="b">
         <v>0</v>
       </c>
       <c r="I145" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="146">
@@ -5824,7 +5812,7 @@
       </c>
       <c r="D146" t="inlineStr">
         <is>
-          <t>Thiago</t>
+          <t>Haaland</t>
         </is>
       </c>
       <c r="E146" t="inlineStr">
@@ -5833,16 +5821,16 @@
         </is>
       </c>
       <c r="F146" t="n">
+        <v>5</v>
+      </c>
+      <c r="G146" t="b">
+        <v>1</v>
+      </c>
+      <c r="H146" t="b">
+        <v>0</v>
+      </c>
+      <c r="I146" t="n">
         <v>2</v>
-      </c>
-      <c r="G146" t="b">
-        <v>0</v>
-      </c>
-      <c r="H146" t="b">
-        <v>0</v>
-      </c>
-      <c r="I146" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="147">
@@ -5861,7 +5849,7 @@
       </c>
       <c r="D147" t="inlineStr">
         <is>
-          <t>Ekitiké</t>
+          <t>Thiago</t>
         </is>
       </c>
       <c r="E147" t="inlineStr">
@@ -5870,13 +5858,13 @@
         </is>
       </c>
       <c r="F147" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G147" t="b">
         <v>0</v>
       </c>
       <c r="H147" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I147" t="n">
         <v>1</v>
@@ -5907,7 +5895,7 @@
         </is>
       </c>
       <c r="F148" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G148" t="b">
         <v>0</v>
@@ -5916,7 +5904,7 @@
         <v>0</v>
       </c>
       <c r="I148" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="149">
@@ -5935,16 +5923,16 @@
       </c>
       <c r="D149" t="inlineStr">
         <is>
-          <t>B.Fernandes</t>
+          <t>Watkins</t>
         </is>
       </c>
       <c r="E149" t="inlineStr">
         <is>
-          <t>MID</t>
+          <t>FWD</t>
         </is>
       </c>
       <c r="F149" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="G149" t="b">
         <v>0</v>
@@ -5953,7 +5941,7 @@
         <v>0</v>
       </c>
       <c r="I149" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="150">
@@ -5972,7 +5960,7 @@
       </c>
       <c r="D150" t="inlineStr">
         <is>
-          <t>Mukiele</t>
+          <t>Estève</t>
         </is>
       </c>
       <c r="E150" t="inlineStr">
@@ -5981,7 +5969,7 @@
         </is>
       </c>
       <c r="F150" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G150" t="b">
         <v>0</v>
@@ -5990,7 +5978,7 @@
         <v>0</v>
       </c>
       <c r="I150" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="151">
@@ -6009,7 +5997,7 @@
       </c>
       <c r="D151" t="inlineStr">
         <is>
-          <t>Estève</t>
+          <t>Guéhi</t>
         </is>
       </c>
       <c r="E151" t="inlineStr">
@@ -6027,7 +6015,7 @@
         <v>0</v>
       </c>
       <c r="I151" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="152">
@@ -6055,7 +6043,7 @@
         </is>
       </c>
       <c r="F152" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G152" t="b">
         <v>0</v>
@@ -6092,7 +6080,7 @@
         </is>
       </c>
       <c r="F153" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G153" t="b">
         <v>0</v>
@@ -6129,7 +6117,7 @@
         </is>
       </c>
       <c r="F154" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G154" t="b">
         <v>0</v>
@@ -6166,7 +6154,7 @@
         </is>
       </c>
       <c r="F155" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="G155" t="b">
         <v>0</v>
@@ -6203,7 +6191,7 @@
         </is>
       </c>
       <c r="F156" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G156" t="b">
         <v>0</v>
@@ -6240,7 +6228,7 @@
         </is>
       </c>
       <c r="F157" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="G157" t="b">
         <v>0</v>
@@ -6277,7 +6265,7 @@
         </is>
       </c>
       <c r="F158" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G158" t="b">
         <v>0</v>
@@ -6314,7 +6302,7 @@
         </is>
       </c>
       <c r="F159" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="G159" t="b">
         <v>0</v>
@@ -6351,7 +6339,7 @@
         </is>
       </c>
       <c r="F160" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G160" t="b">
         <v>1</v>
@@ -6388,7 +6376,7 @@
         </is>
       </c>
       <c r="F161" t="n">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="G161" t="b">
         <v>0</v>
@@ -6462,7 +6450,7 @@
         </is>
       </c>
       <c r="F163" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G163" t="b">
         <v>0</v>
@@ -6536,7 +6524,7 @@
         </is>
       </c>
       <c r="F165" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G165" t="b">
         <v>0</v>
@@ -6573,7 +6561,7 @@
         </is>
       </c>
       <c r="F166" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G166" t="b">
         <v>0</v>
@@ -6610,7 +6598,7 @@
         </is>
       </c>
       <c r="F167" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G167" t="b">
         <v>0</v>
@@ -6638,7 +6626,7 @@
       </c>
       <c r="D168" t="inlineStr">
         <is>
-          <t>J.Timber</t>
+          <t>Konsa</t>
         </is>
       </c>
       <c r="E168" t="inlineStr">
@@ -6647,7 +6635,7 @@
         </is>
       </c>
       <c r="F168" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G168" t="b">
         <v>0</v>
@@ -6675,7 +6663,7 @@
       </c>
       <c r="D169" t="inlineStr">
         <is>
-          <t>Konsa</t>
+          <t>Keane</t>
         </is>
       </c>
       <c r="E169" t="inlineStr">
@@ -6684,7 +6672,7 @@
         </is>
       </c>
       <c r="F169" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="G169" t="b">
         <v>0</v>
@@ -6712,7 +6700,7 @@
       </c>
       <c r="D170" t="inlineStr">
         <is>
-          <t>Van de Ven</t>
+          <t>J.Timber</t>
         </is>
       </c>
       <c r="E170" t="inlineStr">
@@ -6721,7 +6709,7 @@
         </is>
       </c>
       <c r="F170" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G170" t="b">
         <v>0</v>
@@ -6749,7 +6737,7 @@
       </c>
       <c r="D171" t="inlineStr">
         <is>
-          <t>Rogers</t>
+          <t>Anderson</t>
         </is>
       </c>
       <c r="E171" t="inlineStr">
@@ -6758,7 +6746,7 @@
         </is>
       </c>
       <c r="F171" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G171" t="b">
         <v>0</v>
@@ -6786,7 +6774,7 @@
       </c>
       <c r="D172" t="inlineStr">
         <is>
-          <t>Cherki</t>
+          <t>Rogers</t>
         </is>
       </c>
       <c r="E172" t="inlineStr">
@@ -6795,7 +6783,7 @@
         </is>
       </c>
       <c r="F172" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G172" t="b">
         <v>0</v>
@@ -6823,7 +6811,7 @@
       </c>
       <c r="D173" t="inlineStr">
         <is>
-          <t>Rice</t>
+          <t>B.Fernandes</t>
         </is>
       </c>
       <c r="E173" t="inlineStr">
@@ -6832,7 +6820,7 @@
         </is>
       </c>
       <c r="F173" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="G173" t="b">
         <v>0</v>
@@ -6860,7 +6848,7 @@
       </c>
       <c r="D174" t="inlineStr">
         <is>
-          <t>Anderson</t>
+          <t>Rice</t>
         </is>
       </c>
       <c r="E174" t="inlineStr">
@@ -6869,7 +6857,7 @@
         </is>
       </c>
       <c r="F174" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G174" t="b">
         <v>0</v>
@@ -6906,7 +6894,7 @@
         </is>
       </c>
       <c r="F175" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G175" t="b">
         <v>1</v>
@@ -6971,7 +6959,7 @@
       </c>
       <c r="D177" t="inlineStr">
         <is>
-          <t>Watkins</t>
+          <t>João Pedro</t>
         </is>
       </c>
       <c r="E177" t="inlineStr">
@@ -6980,7 +6968,7 @@
         </is>
       </c>
       <c r="F177" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G177" t="b">
         <v>0</v>
@@ -7045,7 +7033,7 @@
       </c>
       <c r="D179" t="inlineStr">
         <is>
-          <t>B.Fernandes</t>
+          <t>Cherki</t>
         </is>
       </c>
       <c r="E179" t="inlineStr">
@@ -7054,7 +7042,7 @@
         </is>
       </c>
       <c r="F179" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="G179" t="b">
         <v>0</v>
@@ -7082,7 +7070,7 @@
       </c>
       <c r="D180" t="inlineStr">
         <is>
-          <t>Keane</t>
+          <t>Van de Ven</t>
         </is>
       </c>
       <c r="E180" t="inlineStr">
@@ -7156,7 +7144,7 @@
       </c>
       <c r="D182" t="inlineStr">
         <is>
-          <t>A.Becker</t>
+          <t>Raya</t>
         </is>
       </c>
       <c r="E182" t="inlineStr">
@@ -7165,7 +7153,7 @@
         </is>
       </c>
       <c r="F182" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="G182" t="b">
         <v>0</v>
@@ -7202,7 +7190,7 @@
         </is>
       </c>
       <c r="F183" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G183" t="b">
         <v>0</v>
@@ -7230,7 +7218,7 @@
       </c>
       <c r="D184" t="inlineStr">
         <is>
-          <t>Cash</t>
+          <t>J.Timber</t>
         </is>
       </c>
       <c r="E184" t="inlineStr">
@@ -7239,7 +7227,7 @@
         </is>
       </c>
       <c r="F184" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G184" t="b">
         <v>0</v>
@@ -7267,7 +7255,7 @@
       </c>
       <c r="D185" t="inlineStr">
         <is>
-          <t>J.Timber</t>
+          <t>Gabriel</t>
         </is>
       </c>
       <c r="E185" t="inlineStr">
@@ -7276,7 +7264,7 @@
         </is>
       </c>
       <c r="F185" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="G185" t="b">
         <v>0</v>
@@ -7304,16 +7292,16 @@
       </c>
       <c r="D186" t="inlineStr">
         <is>
-          <t>Romero</t>
+          <t>Reijnders</t>
         </is>
       </c>
       <c r="E186" t="inlineStr">
         <is>
-          <t>DEF</t>
+          <t>MID</t>
         </is>
       </c>
       <c r="F186" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="G186" t="b">
         <v>0</v>
@@ -7341,16 +7329,16 @@
       </c>
       <c r="D187" t="inlineStr">
         <is>
-          <t>Gabriel</t>
+          <t>Semenyo</t>
         </is>
       </c>
       <c r="E187" t="inlineStr">
         <is>
-          <t>DEF</t>
+          <t>MID</t>
         </is>
       </c>
       <c r="F187" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="G187" t="b">
         <v>0</v>
@@ -7378,7 +7366,7 @@
       </c>
       <c r="D188" t="inlineStr">
         <is>
-          <t>Wilson</t>
+          <t>Gravenberch</t>
         </is>
       </c>
       <c r="E188" t="inlineStr">
@@ -7387,16 +7375,16 @@
         </is>
       </c>
       <c r="F188" t="n">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="G188" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H188" t="b">
         <v>0</v>
       </c>
       <c r="I188" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="189">
@@ -7415,7 +7403,7 @@
       </c>
       <c r="D189" t="inlineStr">
         <is>
-          <t>Gravenberch</t>
+          <t>Wilson</t>
         </is>
       </c>
       <c r="E189" t="inlineStr">
@@ -7424,13 +7412,13 @@
         </is>
       </c>
       <c r="F189" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G189" t="b">
         <v>0</v>
       </c>
       <c r="H189" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I189" t="n">
         <v>1</v>
@@ -7452,7 +7440,7 @@
       </c>
       <c r="D190" t="inlineStr">
         <is>
-          <t>Haaland</t>
+          <t>Thiago</t>
         </is>
       </c>
       <c r="E190" t="inlineStr">
@@ -7461,13 +7449,13 @@
         </is>
       </c>
       <c r="F190" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G190" t="b">
         <v>0</v>
       </c>
       <c r="H190" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I190" t="n">
         <v>1</v>
@@ -7489,7 +7477,7 @@
       </c>
       <c r="D191" t="inlineStr">
         <is>
-          <t>Bowen</t>
+          <t>João Pedro</t>
         </is>
       </c>
       <c r="E191" t="inlineStr">
@@ -7498,16 +7486,16 @@
         </is>
       </c>
       <c r="F191" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G191" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H191" t="b">
         <v>0</v>
       </c>
       <c r="I191" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="192">
@@ -7526,7 +7514,7 @@
       </c>
       <c r="D192" t="inlineStr">
         <is>
-          <t>Thiago</t>
+          <t>Bowen</t>
         </is>
       </c>
       <c r="E192" t="inlineStr">
@@ -7535,7 +7523,7 @@
         </is>
       </c>
       <c r="F192" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="G192" t="b">
         <v>0</v>
@@ -7563,7 +7551,7 @@
       </c>
       <c r="D193" t="inlineStr">
         <is>
-          <t>Raya</t>
+          <t>A.Becker</t>
         </is>
       </c>
       <c r="E193" t="inlineStr">
@@ -7572,7 +7560,7 @@
         </is>
       </c>
       <c r="F193" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G193" t="b">
         <v>0</v>
@@ -7600,16 +7588,16 @@
       </c>
       <c r="D194" t="inlineStr">
         <is>
-          <t>Bruno G.</t>
+          <t>Cash</t>
         </is>
       </c>
       <c r="E194" t="inlineStr">
         <is>
-          <t>MID</t>
+          <t>DEF</t>
         </is>
       </c>
       <c r="F194" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G194" t="b">
         <v>0</v>
@@ -7637,16 +7625,16 @@
       </c>
       <c r="D195" t="inlineStr">
         <is>
-          <t>Semenyo</t>
+          <t>Romero</t>
         </is>
       </c>
       <c r="E195" t="inlineStr">
         <is>
-          <t>MID</t>
+          <t>DEF</t>
         </is>
       </c>
       <c r="F195" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="G195" t="b">
         <v>0</v>
@@ -7674,7 +7662,7 @@
       </c>
       <c r="D196" t="inlineStr">
         <is>
-          <t>Reijnders</t>
+          <t>Bruno G.</t>
         </is>
       </c>
       <c r="E196" t="inlineStr">
@@ -7683,7 +7671,7 @@
         </is>
       </c>
       <c r="F196" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G196" t="b">
         <v>0</v>
@@ -7720,7 +7708,7 @@
         </is>
       </c>
       <c r="F197" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="G197" t="b">
         <v>0</v>
@@ -7748,7 +7736,7 @@
       </c>
       <c r="D198" t="inlineStr">
         <is>
-          <t>Van de Ven</t>
+          <t>Chalobah</t>
         </is>
       </c>
       <c r="E198" t="inlineStr">
@@ -7757,7 +7745,7 @@
         </is>
       </c>
       <c r="F198" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="G198" t="b">
         <v>0</v>
@@ -7794,7 +7782,7 @@
         </is>
       </c>
       <c r="F199" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G199" t="b">
         <v>0</v>
@@ -7831,7 +7819,7 @@
         </is>
       </c>
       <c r="F200" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="G200" t="b">
         <v>0</v>
@@ -7859,7 +7847,7 @@
       </c>
       <c r="D201" t="inlineStr">
         <is>
-          <t>Chalobah</t>
+          <t>Gabriel</t>
         </is>
       </c>
       <c r="E201" t="inlineStr">
@@ -7868,7 +7856,7 @@
         </is>
       </c>
       <c r="F201" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="G201" t="b">
         <v>0</v>
@@ -7905,7 +7893,7 @@
         </is>
       </c>
       <c r="F202" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="G202" t="b">
         <v>0</v>
@@ -7933,7 +7921,7 @@
       </c>
       <c r="D203" t="inlineStr">
         <is>
-          <t>L.Miley</t>
+          <t>Palmer</t>
         </is>
       </c>
       <c r="E203" t="inlineStr">
@@ -7948,7 +7936,7 @@
         <v>0</v>
       </c>
       <c r="H203" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I203" t="n">
         <v>1</v>
@@ -7979,7 +7967,7 @@
         </is>
       </c>
       <c r="F204" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="G204" t="b">
         <v>0</v>
@@ -8007,16 +7995,16 @@
       </c>
       <c r="D205" t="inlineStr">
         <is>
-          <t>Mateta</t>
+          <t>J.Palhinha</t>
         </is>
       </c>
       <c r="E205" t="inlineStr">
         <is>
-          <t>FWD</t>
+          <t>MID</t>
         </is>
       </c>
       <c r="F205" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G205" t="b">
         <v>0</v>
@@ -8053,7 +8041,7 @@
         </is>
       </c>
       <c r="F206" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G206" t="b">
         <v>1</v>
@@ -8127,7 +8115,7 @@
         </is>
       </c>
       <c r="F208" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="G208" t="b">
         <v>0</v>
@@ -8155,7 +8143,7 @@
       </c>
       <c r="D209" t="inlineStr">
         <is>
-          <t>Palmer</t>
+          <t>L.Miley</t>
         </is>
       </c>
       <c r="E209" t="inlineStr">
@@ -8170,7 +8158,7 @@
         <v>0</v>
       </c>
       <c r="H209" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I209" t="n">
         <v>0</v>
@@ -8192,12 +8180,12 @@
       </c>
       <c r="D210" t="inlineStr">
         <is>
-          <t>J.Palhinha</t>
+          <t>Van de Ven</t>
         </is>
       </c>
       <c r="E210" t="inlineStr">
         <is>
-          <t>MID</t>
+          <t>DEF</t>
         </is>
       </c>
       <c r="F210" t="n">
@@ -8229,16 +8217,16 @@
       </c>
       <c r="D211" t="inlineStr">
         <is>
-          <t>Gabriel</t>
+          <t>Mateta</t>
         </is>
       </c>
       <c r="E211" t="inlineStr">
         <is>
-          <t>DEF</t>
+          <t>FWD</t>
         </is>
       </c>
       <c r="F211" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G211" t="b">
         <v>0</v>
@@ -8275,7 +8263,7 @@
         </is>
       </c>
       <c r="F212" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="G212" t="b">
         <v>0</v>
@@ -8303,7 +8291,7 @@
       </c>
       <c r="D213" t="inlineStr">
         <is>
-          <t>J.Timber</t>
+          <t>Tarkowski</t>
         </is>
       </c>
       <c r="E213" t="inlineStr">
@@ -8312,7 +8300,7 @@
         </is>
       </c>
       <c r="F213" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G213" t="b">
         <v>0</v>
@@ -8340,7 +8328,7 @@
       </c>
       <c r="D214" t="inlineStr">
         <is>
-          <t>Van de Ven</t>
+          <t>J.Timber</t>
         </is>
       </c>
       <c r="E214" t="inlineStr">
@@ -8349,7 +8337,7 @@
         </is>
       </c>
       <c r="F214" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G214" t="b">
         <v>0</v>
@@ -8377,7 +8365,7 @@
       </c>
       <c r="D215" t="inlineStr">
         <is>
-          <t>Tarkowski</t>
+          <t>Guéhi</t>
         </is>
       </c>
       <c r="E215" t="inlineStr">
@@ -8386,7 +8374,7 @@
         </is>
       </c>
       <c r="F215" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G215" t="b">
         <v>0</v>
@@ -8414,7 +8402,7 @@
       </c>
       <c r="D216" t="inlineStr">
         <is>
-          <t>Guéhi</t>
+          <t>Senesi</t>
         </is>
       </c>
       <c r="E216" t="inlineStr">
@@ -8423,7 +8411,7 @@
         </is>
       </c>
       <c r="F216" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G216" t="b">
         <v>0</v>
@@ -8451,7 +8439,7 @@
       </c>
       <c r="D217" t="inlineStr">
         <is>
-          <t>Ndiaye</t>
+          <t>Enzo</t>
         </is>
       </c>
       <c r="E217" t="inlineStr">
@@ -8460,7 +8448,7 @@
         </is>
       </c>
       <c r="F217" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="G217" t="b">
         <v>0</v>
@@ -8488,7 +8476,7 @@
       </c>
       <c r="D218" t="inlineStr">
         <is>
-          <t>Enzo</t>
+          <t>Rice</t>
         </is>
       </c>
       <c r="E218" t="inlineStr">
@@ -8497,7 +8485,7 @@
         </is>
       </c>
       <c r="F218" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="G218" t="b">
         <v>0</v>
@@ -8525,7 +8513,7 @@
       </c>
       <c r="D219" t="inlineStr">
         <is>
-          <t>Rice</t>
+          <t>Ndiaye</t>
         </is>
       </c>
       <c r="E219" t="inlineStr">
@@ -8534,7 +8522,7 @@
         </is>
       </c>
       <c r="F219" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G219" t="b">
         <v>0</v>
@@ -8562,16 +8550,16 @@
       </c>
       <c r="D220" t="inlineStr">
         <is>
-          <t>Woltemade</t>
+          <t>Semenyo</t>
         </is>
       </c>
       <c r="E220" t="inlineStr">
         <is>
-          <t>FWD</t>
+          <t>MID</t>
         </is>
       </c>
       <c r="F220" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="G220" t="b">
         <v>0</v>
@@ -8608,7 +8596,7 @@
         </is>
       </c>
       <c r="F221" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G221" t="b">
         <v>1</v>
@@ -8636,7 +8624,7 @@
       </c>
       <c r="D222" t="inlineStr">
         <is>
-          <t>Ekitiké</t>
+          <t>João Pedro</t>
         </is>
       </c>
       <c r="E222" t="inlineStr">
@@ -8645,7 +8633,7 @@
         </is>
       </c>
       <c r="F222" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="G222" t="b">
         <v>0</v>
@@ -8682,7 +8670,7 @@
         </is>
       </c>
       <c r="F223" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G223" t="b">
         <v>0</v>
@@ -8710,16 +8698,16 @@
       </c>
       <c r="D224" t="inlineStr">
         <is>
-          <t>Xhaka</t>
+          <t>Thiago</t>
         </is>
       </c>
       <c r="E224" t="inlineStr">
         <is>
-          <t>MID</t>
+          <t>FWD</t>
         </is>
       </c>
       <c r="F224" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G224" t="b">
         <v>0</v>
@@ -8747,7 +8735,7 @@
       </c>
       <c r="D225" t="inlineStr">
         <is>
-          <t>Bruno G.</t>
+          <t>Xhaka</t>
         </is>
       </c>
       <c r="E225" t="inlineStr">
@@ -8784,7 +8772,7 @@
       </c>
       <c r="D226" t="inlineStr">
         <is>
-          <t>Senesi</t>
+          <t>Van de Ven</t>
         </is>
       </c>
       <c r="E226" t="inlineStr">
@@ -8793,7 +8781,7 @@
         </is>
       </c>
       <c r="F226" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G226" t="b">
         <v>0</v>
@@ -8830,7 +8818,7 @@
         </is>
       </c>
       <c r="F227" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="G227" t="b">
         <v>0</v>
@@ -8867,7 +8855,7 @@
         </is>
       </c>
       <c r="F228" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G228" t="b">
         <v>0</v>
@@ -8904,7 +8892,7 @@
         </is>
       </c>
       <c r="F229" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G229" t="b">
         <v>0</v>
@@ -8932,7 +8920,7 @@
       </c>
       <c r="D230" t="inlineStr">
         <is>
-          <t>Andersen</t>
+          <t>Senesi</t>
         </is>
       </c>
       <c r="E230" t="inlineStr">
@@ -9015,7 +9003,7 @@
         </is>
       </c>
       <c r="F232" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G232" t="b">
         <v>0</v>
@@ -9043,7 +9031,7 @@
       </c>
       <c r="D233" t="inlineStr">
         <is>
-          <t>Foden</t>
+          <t>B.Fernandes</t>
         </is>
       </c>
       <c r="E233" t="inlineStr">
@@ -9052,16 +9040,16 @@
         </is>
       </c>
       <c r="F233" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="G233" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H233" t="b">
         <v>0</v>
       </c>
       <c r="I233" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="234">
@@ -9089,7 +9077,7 @@
         </is>
       </c>
       <c r="F234" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G234" t="b">
         <v>0</v>
@@ -9163,16 +9151,16 @@
         </is>
       </c>
       <c r="F236" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G236" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H236" t="b">
         <v>0</v>
       </c>
       <c r="I236" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="237">
@@ -9200,7 +9188,7 @@
         </is>
       </c>
       <c r="F237" t="n">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="G237" t="b">
         <v>0</v>
@@ -9237,7 +9225,7 @@
         </is>
       </c>
       <c r="F238" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G238" t="b">
         <v>0</v>
@@ -9311,7 +9299,7 @@
         </is>
       </c>
       <c r="F240" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="G240" t="b">
         <v>0</v>
@@ -9339,7 +9327,7 @@
       </c>
       <c r="D241" t="inlineStr">
         <is>
-          <t>Senesi</t>
+          <t>Andersen</t>
         </is>
       </c>
       <c r="E241" t="inlineStr">
@@ -9348,7 +9336,7 @@
         </is>
       </c>
       <c r="F241" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G241" t="b">
         <v>0</v>
@@ -9385,7 +9373,7 @@
         </is>
       </c>
       <c r="F242" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G242" t="b">
         <v>0</v>
@@ -9422,7 +9410,7 @@
         </is>
       </c>
       <c r="F243" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="G243" t="b">
         <v>0</v>
@@ -9459,7 +9447,7 @@
         </is>
       </c>
       <c r="F244" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="G244" t="b">
         <v>0</v>
@@ -9487,7 +9475,7 @@
       </c>
       <c r="D245" t="inlineStr">
         <is>
-          <t>Pedro Porro</t>
+          <t>Muñoz</t>
         </is>
       </c>
       <c r="E245" t="inlineStr">
@@ -9496,7 +9484,7 @@
         </is>
       </c>
       <c r="F245" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G245" t="b">
         <v>0</v>
@@ -9524,12 +9512,12 @@
       </c>
       <c r="D246" t="inlineStr">
         <is>
-          <t>Muñoz</t>
+          <t>Reijnders</t>
         </is>
       </c>
       <c r="E246" t="inlineStr">
         <is>
-          <t>DEF</t>
+          <t>MID</t>
         </is>
       </c>
       <c r="F246" t="n">
@@ -9561,7 +9549,7 @@
       </c>
       <c r="D247" t="inlineStr">
         <is>
-          <t>Reijnders</t>
+          <t>P.M.Sarr</t>
         </is>
       </c>
       <c r="E247" t="inlineStr">
@@ -9570,7 +9558,7 @@
         </is>
       </c>
       <c r="F247" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G247" t="b">
         <v>0</v>
@@ -9598,7 +9586,7 @@
       </c>
       <c r="D248" t="inlineStr">
         <is>
-          <t>Mitoma</t>
+          <t>Iwobi</t>
         </is>
       </c>
       <c r="E248" t="inlineStr">
@@ -9635,7 +9623,7 @@
       </c>
       <c r="D249" t="inlineStr">
         <is>
-          <t>Iwobi</t>
+          <t>Mitoma</t>
         </is>
       </c>
       <c r="E249" t="inlineStr">
@@ -9681,7 +9669,7 @@
         </is>
       </c>
       <c r="F250" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G250" t="b">
         <v>1</v>
@@ -9718,7 +9706,7 @@
         </is>
       </c>
       <c r="F251" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="G251" t="b">
         <v>0</v>
@@ -9755,7 +9743,7 @@
         </is>
       </c>
       <c r="F252" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G252" t="b">
         <v>0</v>
@@ -9857,7 +9845,7 @@
       </c>
       <c r="D255" t="inlineStr">
         <is>
-          <t>P.M.Sarr</t>
+          <t>Kudus</t>
         </is>
       </c>
       <c r="E255" t="inlineStr">
@@ -9894,12 +9882,12 @@
       </c>
       <c r="D256" t="inlineStr">
         <is>
-          <t>Kudus</t>
+          <t>Pedro Porro</t>
         </is>
       </c>
       <c r="E256" t="inlineStr">
         <is>
-          <t>MID</t>
+          <t>DEF</t>
         </is>
       </c>
       <c r="F256" t="n">
@@ -9931,7 +9919,7 @@
       </c>
       <c r="D257" t="inlineStr">
         <is>
-          <t>Leno</t>
+          <t>Raya</t>
         </is>
       </c>
       <c r="E257" t="inlineStr">
@@ -9940,7 +9928,7 @@
         </is>
       </c>
       <c r="F257" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G257" t="b">
         <v>0</v>
@@ -9968,7 +9956,7 @@
       </c>
       <c r="D258" t="inlineStr">
         <is>
-          <t>J.Timber</t>
+          <t>Tarkowski</t>
         </is>
       </c>
       <c r="E258" t="inlineStr">
@@ -9977,7 +9965,7 @@
         </is>
       </c>
       <c r="F258" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G258" t="b">
         <v>0</v>
@@ -10005,7 +9993,7 @@
       </c>
       <c r="D259" t="inlineStr">
         <is>
-          <t>Alderete</t>
+          <t>James</t>
         </is>
       </c>
       <c r="E259" t="inlineStr">
@@ -10042,7 +10030,7 @@
       </c>
       <c r="D260" t="inlineStr">
         <is>
-          <t>Virgil</t>
+          <t>Gabriel</t>
         </is>
       </c>
       <c r="E260" t="inlineStr">
@@ -10051,7 +10039,7 @@
         </is>
       </c>
       <c r="F260" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G260" t="b">
         <v>0</v>
@@ -10079,16 +10067,16 @@
       </c>
       <c r="D261" t="inlineStr">
         <is>
-          <t>Rice</t>
+          <t>Senesi</t>
         </is>
       </c>
       <c r="E261" t="inlineStr">
         <is>
-          <t>MID</t>
+          <t>DEF</t>
         </is>
       </c>
       <c r="F261" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="G261" t="b">
         <v>0</v>
@@ -10116,7 +10104,7 @@
       </c>
       <c r="D262" t="inlineStr">
         <is>
-          <t>Wilson</t>
+          <t>Rice</t>
         </is>
       </c>
       <c r="E262" t="inlineStr">
@@ -10125,7 +10113,7 @@
         </is>
       </c>
       <c r="F262" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="G262" t="b">
         <v>0</v>
@@ -10162,13 +10150,13 @@
         </is>
       </c>
       <c r="F263" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G263" t="b">
         <v>0</v>
       </c>
       <c r="H263" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I263" t="n">
         <v>1</v>
@@ -10227,16 +10215,16 @@
       </c>
       <c r="D265" t="inlineStr">
         <is>
-          <t>Ekitiké</t>
+          <t>B.Fernandes</t>
         </is>
       </c>
       <c r="E265" t="inlineStr">
         <is>
-          <t>FWD</t>
+          <t>MID</t>
         </is>
       </c>
       <c r="F265" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="G265" t="b">
         <v>0</v>
@@ -10264,7 +10252,7 @@
       </c>
       <c r="D266" t="inlineStr">
         <is>
-          <t>Thiago</t>
+          <t>João Pedro</t>
         </is>
       </c>
       <c r="E266" t="inlineStr">
@@ -10273,16 +10261,16 @@
         </is>
       </c>
       <c r="F266" t="n">
+        <v>10</v>
+      </c>
+      <c r="G266" t="b">
+        <v>1</v>
+      </c>
+      <c r="H266" t="b">
+        <v>0</v>
+      </c>
+      <c r="I266" t="n">
         <v>2</v>
-      </c>
-      <c r="G266" t="b">
-        <v>0</v>
-      </c>
-      <c r="H266" t="b">
-        <v>0</v>
-      </c>
-      <c r="I266" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="267">
@@ -10310,16 +10298,16 @@
         </is>
       </c>
       <c r="F267" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G267" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H267" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I267" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="268">
@@ -10338,7 +10326,7 @@
       </c>
       <c r="D268" t="inlineStr">
         <is>
-          <t>Valdimarsson</t>
+          <t>Kelleher</t>
         </is>
       </c>
       <c r="E268" t="inlineStr">
@@ -10347,7 +10335,7 @@
         </is>
       </c>
       <c r="F268" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="G268" t="b">
         <v>0</v>
@@ -10375,7 +10363,7 @@
       </c>
       <c r="D269" t="inlineStr">
         <is>
-          <t>Bruno G.</t>
+          <t>Wilson</t>
         </is>
       </c>
       <c r="E269" t="inlineStr">
@@ -10384,7 +10372,7 @@
         </is>
       </c>
       <c r="F269" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G269" t="b">
         <v>0</v>
@@ -10412,16 +10400,16 @@
       </c>
       <c r="D270" t="inlineStr">
         <is>
-          <t>Senesi</t>
+          <t>Kroupi.Jr</t>
         </is>
       </c>
       <c r="E270" t="inlineStr">
         <is>
-          <t>DEF</t>
+          <t>FWD</t>
         </is>
       </c>
       <c r="F270" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="G270" t="b">
         <v>0</v>
@@ -10449,7 +10437,7 @@
       </c>
       <c r="D271" t="inlineStr">
         <is>
-          <t>Hincapie</t>
+          <t>Guéhi</t>
         </is>
       </c>
       <c r="E271" t="inlineStr">
@@ -10458,7 +10446,7 @@
         </is>
       </c>
       <c r="F271" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G271" t="b">
         <v>0</v>
@@ -10486,7 +10474,7 @@
       </c>
       <c r="D272" t="inlineStr">
         <is>
-          <t>Pickford</t>
+          <t>Sánchez</t>
         </is>
       </c>
       <c r="E272" t="inlineStr">
@@ -10495,7 +10483,7 @@
         </is>
       </c>
       <c r="F272" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G272" t="b">
         <v>0</v>
@@ -10532,7 +10520,7 @@
         </is>
       </c>
       <c r="F273" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="G273" t="b">
         <v>0</v>
@@ -10569,7 +10557,7 @@
         </is>
       </c>
       <c r="F274" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G274" t="b">
         <v>0</v>
@@ -10597,7 +10585,7 @@
       </c>
       <c r="D275" t="inlineStr">
         <is>
-          <t>Hall</t>
+          <t>Guéhi</t>
         </is>
       </c>
       <c r="E275" t="inlineStr">
@@ -10606,7 +10594,7 @@
         </is>
       </c>
       <c r="F275" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G275" t="b">
         <v>0</v>
@@ -10643,7 +10631,7 @@
         </is>
       </c>
       <c r="F276" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="G276" t="b">
         <v>0</v>
@@ -10680,7 +10668,7 @@
         </is>
       </c>
       <c r="F277" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G277" t="b">
         <v>0</v>
@@ -10717,7 +10705,7 @@
         </is>
       </c>
       <c r="F278" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G278" t="b">
         <v>0</v>
@@ -10754,7 +10742,7 @@
         </is>
       </c>
       <c r="F279" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G279" t="b">
         <v>0</v>
@@ -10791,7 +10779,7 @@
         </is>
       </c>
       <c r="F280" t="n">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="G280" t="b">
         <v>0</v>
@@ -10828,7 +10816,7 @@
         </is>
       </c>
       <c r="F281" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G281" t="b">
         <v>1</v>
@@ -10893,7 +10881,7 @@
       </c>
       <c r="D283" t="inlineStr">
         <is>
-          <t>Sánchez</t>
+          <t>Pickford</t>
         </is>
       </c>
       <c r="E283" t="inlineStr">
@@ -10902,7 +10890,7 @@
         </is>
       </c>
       <c r="F283" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G283" t="b">
         <v>0</v>
@@ -10967,7 +10955,7 @@
       </c>
       <c r="D285" t="inlineStr">
         <is>
-          <t>Guéhi</t>
+          <t>Hall</t>
         </is>
       </c>
       <c r="E285" t="inlineStr">
@@ -10976,7 +10964,7 @@
         </is>
       </c>
       <c r="F285" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G285" t="b">
         <v>0</v>
@@ -11050,7 +11038,7 @@
         </is>
       </c>
       <c r="F287" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="G287" t="b">
         <v>0</v>
@@ -11087,7 +11075,7 @@
         </is>
       </c>
       <c r="F288" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="G288" t="b">
         <v>0</v>
@@ -11124,7 +11112,7 @@
         </is>
       </c>
       <c r="F289" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="G289" t="b">
         <v>0</v>
@@ -11161,7 +11149,7 @@
         </is>
       </c>
       <c r="F290" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="G290" t="b">
         <v>0</v>
@@ -11198,7 +11186,7 @@
         </is>
       </c>
       <c r="F291" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G291" t="b">
         <v>0</v>
@@ -11235,7 +11223,7 @@
         </is>
       </c>
       <c r="F292" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="G292" t="b">
         <v>0</v>
@@ -11272,7 +11260,7 @@
         </is>
       </c>
       <c r="F293" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G293" t="b">
         <v>0</v>
@@ -11346,7 +11334,7 @@
         </is>
       </c>
       <c r="F295" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G295" t="b">
         <v>1</v>
@@ -11457,7 +11445,7 @@
         </is>
       </c>
       <c r="F298" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G298" t="b">
         <v>0</v>
@@ -11531,7 +11519,7 @@
         </is>
       </c>
       <c r="F300" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G300" t="b">
         <v>0</v>

</xml_diff>